<commit_message>
fixing metadata for frontispieces
</commit_message>
<xml_diff>
--- a/clo-angular/src/assets/albums/fullsize/album_01/Volume1.xlsx
+++ b/clo-angular/src/assets/albums/fullsize/album_01/Volume1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stella/clo3/clo-angular/src/assets/albums/fullsize/album_01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5C993E-7129-6547-9BEC-235EB4DABFE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9148E8B1-45B5-1945-96B0-2788B6438973}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,7 +470,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">

</xml_diff>